<commit_message>
update Yilin Wang diary
</commit_message>
<xml_diff>
--- a/diaries/diary-Yilin Wang.xlsx
+++ b/diaries/diary-Yilin Wang.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlwan\Documents\Study\reverse_engineering\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47881934-29D0-459D-8AFD-E18678263603}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F27EDD-51D4-4479-A3B7-5B4DA5FCE153}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="171">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -352,6 +352,224 @@
     <t>Reading code is a slow process.
 Codes are natural not to understand.
 Needs to worry about what feature to implement and make the pull request.</t>
+  </si>
+  <si>
+    <t>09:00 AM - 01:00 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revise what we learned on the last lecture.
+1. Learn 3 KEP
+2. how to extract architecture from the source code.
+3. how to identify social context of the project.
+</t>
+  </si>
+  <si>
+    <t>Three KEP are how things work, address knowledge deficiencies, design elegant attractions.</t>
+  </si>
+  <si>
+    <t>Jpacman is a really interesting project. My group just make an assumption that game is definitely a MVC architecture and find evidence. UML is a helpful tool, but maybe not helpful when project is larger. Because classes are nested together</t>
+  </si>
+  <si>
+    <t>20:00 PM - 01:00 AM</t>
+  </si>
+  <si>
+    <t>Start working on homework this week.Try to find some basic codes style or becon to decide the architecture. Try to find something useful online.</t>
+  </si>
+  <si>
+    <t>To be honest, try to understand architecture without any assistance is unrealistic for me. The project is so large and everything is nested together. Sometimes, we need to follow the control flow for 10 steps but still can't find the implemetation, and I could not understand this process.</t>
+  </si>
+  <si>
+    <t>I guess I should search more information online so that I could understand the architecture of this project.</t>
+  </si>
+  <si>
+    <t>Not Good.</t>
+  </si>
+  <si>
+    <t>19:00 PM - 02:00 AM</t>
+  </si>
+  <si>
+    <t>Finish the architecture analysis and work on the PR and commits</t>
+  </si>
+  <si>
+    <t>Based on some articles, spring-boot inherits the layered architecture from spring.I managed to find some patterns fit in this architecture, but not all of them, the main reason is that some layer are in the spring , not spring boot.</t>
+  </si>
+  <si>
+    <t>Found some useful articles about spring-boot architecture, spring actually. This is interesting that spring boot is just a wrap of spring, I'm wondering that if we take spring away, is there an architecture left? Maybe it's not a good idea to analyze springboot without spring</t>
+  </si>
+  <si>
+    <t>tired.</t>
+  </si>
+  <si>
+    <t>20:00 PM - 02:30 AM</t>
+  </si>
+  <si>
+    <t>Finish the homework and make a pull request.</t>
+  </si>
+  <si>
+    <t>Just reviewing those pull request, we could learn a lot. For spring boot, most of the pull requests are actually made by offcial developers, so history of spring boot just lies in the pull requests. Commits are pretty frequent, they are vary diligent.</t>
+  </si>
+  <si>
+    <t>Just occurred to me that I could not understand what's the pul request are really talking about. I believe that if I have any previous experience with spring boot, reading the source code could be more instructive and helpful.</t>
+  </si>
+  <si>
+    <t>17:00 PM - 20:00 PM</t>
+  </si>
+  <si>
+    <t>Learn the design patterns and from senior engineers</t>
+  </si>
+  <si>
+    <t>1. Invest now and save time later
+2. varieties of design pattern</t>
+  </si>
+  <si>
+    <t>Design patterns are really important, it could help us produce more structral and more elegant codes. Among this semester, I already found some patterns in the spring boot. It's interesting that some classes are structural similar, I guess this is due to the pattern.</t>
+  </si>
+  <si>
+    <t>Average. Homework is a lot.</t>
+  </si>
+  <si>
+    <t>19:00 PM - 00:30 AM</t>
+  </si>
+  <si>
+    <t>Find five design patterns
+Understand their definitions and understand their implementation.</t>
+  </si>
+  <si>
+    <t>Found the abstractfactory pattern, but I found that it is not quite like the definition, and the factory has so many layers and implementations, I spent a lot of time trying to find where and how to create an instance, but as I follows, the codes became more and more intrigue and I have to say I usually got lost. So I just finished this pattern and adapter pattern. I found this pattern when I did homework2.</t>
+  </si>
+  <si>
+    <t>Maybe sometimes real pattern is not exactly same with the definition? It's hard to say but when diving deep to the codes deeper, it's more difficult to follow the developers ideas and understand the flow of spring boot.</t>
+  </si>
+  <si>
+    <t>Tired</t>
+  </si>
+  <si>
+    <t>13:00 PM - 22:30 AM</t>
+  </si>
+  <si>
+    <t>Find remaining patterns and finish the writeup</t>
+  </si>
+  <si>
+    <t>Found the singleton, builder and observer pattern.buider pattern is quite easy and starightforward, but singleton is kind of hard to understand.</t>
+  </si>
+  <si>
+    <t>It's interesting that when I did my homework2, I noticed that there is a builder class inside a class, and I googled the reason, and now I know that this is the builder pattern.Pretty excited about it!</t>
+  </si>
+  <si>
+    <t>12:00 - 17:30PM</t>
+  </si>
+  <si>
+    <t>Find an issue and make a PR</t>
+  </si>
+  <si>
+    <t>This is really hard.Spring-boot is a very stable framework and finding even a trivial thing is difficult. I notice that there is a redundancy in the if statement, this should be our key to the homework.</t>
+  </si>
+  <si>
+    <t>Trying to come up with some updates about spring boot is so hard. And I feel a little bit shy about submittingPR. The reason is all recently PRs are made by official developers and our PR is really trivial.</t>
+  </si>
+  <si>
+    <t>Learn more about KEP, testing, and guests!</t>
+  </si>
+  <si>
+    <t>Weihuan Fu, Tianyu Qi, Xiaolue Peng</t>
+  </si>
+  <si>
+    <t>This class is really fruitful! Learning from others' PR contents is interesting and instructive, and broaden my ideas about it. And We found that our PR got merged. This is really exciting because I never expected that our PR would be merged. A strong sense of achivement! And the visitors are great! Their lecture is so interesting and it reminds me of my bachelor times, because my major was EE and worked with these stuff everyday! 
+And to identify a framework, there is a line X.start(). Very incisive.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To make a contribution to an open source project is really exciting, even if only a trivial PR.
+I remembered that my Physical teacher told us you should not only require stuff from Internet, but also make a contribution. And today I do. I'm really glad that I found that little problem and make a PR bravely. </t>
+  </si>
+  <si>
+    <t>Terrific!</t>
+  </si>
+  <si>
+    <t>20:00 PM - 23:00 PM</t>
+  </si>
+  <si>
+    <t>Started browsing the issue section and tried to find something on my level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I literally can not find any open issues that I could understand. As I said before, spring booy is a well developed framework for large industry application. And developers are willing to help. So what's left in the open issues is really hard to address. As a matter of fact, I even could not understand the problems themselves. </t>
+  </si>
+  <si>
+    <t>Just very disappointed about myself and worried about this homework.I believe that this could be easier if I have any experience with spring boot. Right now I'm very desperate and I don't think that I have the ability to address an open issue.</t>
+  </si>
+  <si>
+    <t>Bad.</t>
+  </si>
+  <si>
+    <t>19:00 PM - 23:00 PM</t>
+  </si>
+  <si>
+    <t>And another reason this homework is so hard is that many open issues are about their own applications built on the spring boot, not the spring boot itself. And their applications are even larger because most of applications are industry levels. There is no way for me to solve their problems even only for understanding their problems.</t>
+  </si>
+  <si>
+    <t>A fruitless day. With other finals, I'm really tired and worried. I have to say that spring boot really get my interests and I decided to learn it more systematicly. Trying to build something with spring boot probably benefits more.</t>
+  </si>
+  <si>
+    <t>Keep searching for any open issues within my capability. 
+Only thing I found is about inputstream, which at least I could understand what he's talking about.</t>
+  </si>
+  <si>
+    <t>Learn more about KEP and wrap up</t>
+  </si>
+  <si>
+    <t>This is the last lecture. This course is really helpful and useful. I never imagine that I would read so many codes.But I did. For today, keep learning is really a good suggestion for me. And I will keep read code by the guideline.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average. </t>
+  </si>
+  <si>
+    <t>Learn more about enduring principles.
+Respect the code.
+And Decide that we will try to solve the issue mentioned earlier.</t>
+  </si>
+  <si>
+    <t>17:00 PM - 2:00 AM</t>
+  </si>
+  <si>
+    <t>Dig more about JarWriter and try to find some techniques so that we could address this issue.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This class is relatively easy to understand compared with other classes. However, Jar Writer calls buffer writing function and it seems unlikely to work around this. </t>
+  </si>
+  <si>
+    <t>Tired.</t>
+  </si>
+  <si>
+    <t>The Inputstream function looks fine, and this probably the best it could get except that we override the bufferinput function. But it's definitely impossible for us to write a better function than Oracle genius. Gotta find something else.Maybe Concurrency?</t>
+  </si>
+  <si>
+    <t>11:00 AM - 20:00 PM</t>
+  </si>
+  <si>
+    <t>Write Testcases and finish that report.</t>
+  </si>
+  <si>
+    <t>Learned how to write testcase to a database. It's not just set a name and get the name, but to create a MongoClient database, and get the credentials from the real database. By writing this testcase, I got a better sense of how MongoDB works in spring boot.</t>
+  </si>
+  <si>
+    <t>Some thoughts about the Jar Writer. Is it possible that Jar writer takes too much memory because the file is too large? If we trunk the file into small pieces, the memory use could be better?</t>
+  </si>
+  <si>
+    <t>Reflective</t>
+  </si>
+  <si>
+    <t>11:00 AM - 23:00 PM</t>
+  </si>
+  <si>
+    <t>Not sure if we are on the right track, but we are gonna give a try. Finish writing trunk function and combine it with input stream. Even if this idea doesn't work out, we could learn something about file trunking!</t>
+  </si>
+  <si>
+    <t>Successfully trunk the files, and finished other two reports.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I just noticed that developers mark this to the milestone and will fix this issue in the future. So I will definitely stay tuned and see how they deal with this problem. This is a good way to learn! And I purchased a Udemy course about spring and spring boot, I will learn more about how to use this framework in the spring break. </t>
+  </si>
+  <si>
+    <t>Tired. Wish myself luck in the final</t>
   </si>
 </sst>
 </file>
@@ -505,7 +723,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -575,6 +793,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -894,21 +1115,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
-  <dimension ref="A1:G126"/>
+  <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="B42" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.26953125" customWidth="1"/>
-    <col min="2" max="3" width="34.6328125" customWidth="1"/>
-    <col min="4" max="6" width="34.6328125" style="12" customWidth="1"/>
-    <col min="7" max="7" width="34.6328125" customWidth="1"/>
+    <col min="1" max="1" width="13.21875" customWidth="1"/>
+    <col min="2" max="3" width="34.6640625" customWidth="1"/>
+    <col min="4" max="6" width="34.6640625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -919,7 +1140,7 @@
       <c r="F1" s="23"/>
       <c r="G1" s="23"/>
     </row>
-    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -928,7 +1149,7 @@
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
     </row>
-    <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -937,7 +1158,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -950,7 +1171,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -963,7 +1184,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -976,7 +1197,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -985,7 +1206,7 @@
       <c r="F7" s="10"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -994,7 +1215,7 @@
       <c r="F8" s="11"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>4</v>
       </c>
@@ -1017,7 +1238,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="15">
         <v>43839</v>
       </c>
@@ -1040,7 +1261,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="78" x14ac:dyDescent="0.3">
       <c r="A11" s="15">
         <v>43846</v>
       </c>
@@ -1063,7 +1284,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A12" s="15">
         <v>43853</v>
       </c>
@@ -1086,7 +1307,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="15">
         <v>43856</v>
       </c>
@@ -1109,7 +1330,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="15">
         <v>43858</v>
       </c>
@@ -1132,7 +1353,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A15" s="15">
         <v>43860</v>
       </c>
@@ -1155,7 +1376,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="93" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A16" s="15">
         <v>43861</v>
       </c>
@@ -1178,7 +1399,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A17" s="15">
         <v>43863</v>
       </c>
@@ -1201,7 +1422,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A18" s="21">
         <v>43865</v>
       </c>
@@ -1224,7 +1445,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="155" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="156" x14ac:dyDescent="0.3">
       <c r="A19" s="15">
         <v>43867</v>
       </c>
@@ -1247,7 +1468,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A20" s="15">
         <v>43868</v>
       </c>
@@ -1270,7 +1491,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A21" s="15">
         <v>43869</v>
       </c>
@@ -1293,7 +1514,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A22" s="15">
         <v>43871</v>
       </c>
@@ -1316,7 +1537,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="93" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A23" s="15">
         <v>43873</v>
       </c>
@@ -1339,7 +1560,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A24" s="15">
         <v>43874</v>
       </c>
@@ -1362,7 +1583,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A25" s="15">
         <v>43876</v>
       </c>
@@ -1385,7 +1606,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A26" s="15">
         <v>43877</v>
       </c>
@@ -1408,7 +1629,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="139.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="156" x14ac:dyDescent="0.3">
       <c r="A27" s="15">
         <v>43879</v>
       </c>
@@ -1429,7 +1650,7 @@
       </c>
       <c r="G27" s="19"/>
     </row>
-    <row r="28" spans="1:7" ht="139.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="140.4" x14ac:dyDescent="0.3">
       <c r="A28" s="15">
         <v>43880</v>
       </c>
@@ -1452,7 +1673,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A29" s="15">
         <v>43881</v>
       </c>
@@ -1475,143 +1696,353 @@
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="7"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="7"/>
-    </row>
-    <row r="33" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="7"/>
-    </row>
-    <row r="34" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="7"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="7"/>
-    </row>
-    <row r="37" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="7"/>
-    </row>
-    <row r="38" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="7"/>
-    </row>
-    <row r="39" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="7"/>
-    </row>
-    <row r="40" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="7"/>
-    </row>
-    <row r="41" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="7"/>
-    </row>
-    <row r="42" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="7"/>
-    </row>
-    <row r="43" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="7"/>
-    </row>
-    <row r="44" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="7"/>
-    </row>
-    <row r="45" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="6"/>
+    <row r="30" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="15">
+        <v>43883</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="G30" s="19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="15">
+        <v>43884</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="G31" s="19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="A32" s="15">
+        <v>43885</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="G32" s="19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="15">
+        <v>43887</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G33" s="19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="15">
+        <v>43888</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="F34" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="G34" s="19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="202.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="15">
+        <v>43890</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="G35" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="15">
+        <v>43891</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="F36" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="G36" s="19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="15">
+        <v>43893</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="G37" s="19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="249.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="15">
+        <v>43895</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="G38" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="156" x14ac:dyDescent="0.3">
+      <c r="A39" s="15">
+        <v>43896</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="G39" s="19" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="171.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="15">
+        <v>43899</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="G40" s="19" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A41" s="15">
+        <v>43902</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="F41" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="G41" s="19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="15">
+        <v>43903</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="G42" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="15">
+        <v>43905</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="E43" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="F43" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="G43" s="19" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="156" x14ac:dyDescent="0.3">
+      <c r="A44" s="15">
+        <v>43906</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="F44" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="G44" s="19" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="24"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
       <c r="D45" s="9"/>
@@ -1619,8 +2050,8 @@
       <c r="F45" s="9"/>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="6"/>
+    <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="24"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
       <c r="D46" s="9"/>
@@ -1628,8 +2059,8 @@
       <c r="F46" s="9"/>
       <c r="G46" s="7"/>
     </row>
-    <row r="47" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="6"/>
+    <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="24"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
       <c r="D47" s="9"/>
@@ -1637,7 +2068,7 @@
       <c r="F47" s="9"/>
       <c r="G47" s="7"/>
     </row>
-    <row r="48" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -1646,7 +2077,7 @@
       <c r="F48" s="9"/>
       <c r="G48" s="7"/>
     </row>
-    <row r="49" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -1655,7 +2086,7 @@
       <c r="F49" s="9"/>
       <c r="G49" s="7"/>
     </row>
-    <row r="50" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
@@ -1664,7 +2095,7 @@
       <c r="F50" s="9"/>
       <c r="G50" s="7"/>
     </row>
-    <row r="51" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -1673,7 +2104,7 @@
       <c r="F51" s="9"/>
       <c r="G51" s="7"/>
     </row>
-    <row r="52" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
@@ -1682,7 +2113,7 @@
       <c r="F52" s="9"/>
       <c r="G52" s="7"/>
     </row>
-    <row r="53" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -1691,7 +2122,7 @@
       <c r="F53" s="9"/>
       <c r="G53" s="7"/>
     </row>
-    <row r="54" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -1700,7 +2131,7 @@
       <c r="F54" s="9"/>
       <c r="G54" s="7"/>
     </row>
-    <row r="55" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -1709,7 +2140,7 @@
       <c r="F55" s="9"/>
       <c r="G55" s="7"/>
     </row>
-    <row r="56" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -1718,7 +2149,7 @@
       <c r="F56" s="9"/>
       <c r="G56" s="7"/>
     </row>
-    <row r="57" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
@@ -1727,7 +2158,7 @@
       <c r="F57" s="9"/>
       <c r="G57" s="7"/>
     </row>
-    <row r="58" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -1736,7 +2167,7 @@
       <c r="F58" s="9"/>
       <c r="G58" s="7"/>
     </row>
-    <row r="59" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
@@ -1745,7 +2176,7 @@
       <c r="F59" s="9"/>
       <c r="G59" s="7"/>
     </row>
-    <row r="60" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
@@ -1754,7 +2185,7 @@
       <c r="F60" s="9"/>
       <c r="G60" s="7"/>
     </row>
-    <row r="61" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
@@ -1763,7 +2194,7 @@
       <c r="F61" s="9"/>
       <c r="G61" s="7"/>
     </row>
-    <row r="62" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
@@ -1772,7 +2203,7 @@
       <c r="F62" s="9"/>
       <c r="G62" s="7"/>
     </row>
-    <row r="63" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
@@ -1781,7 +2212,7 @@
       <c r="F63" s="9"/>
       <c r="G63" s="7"/>
     </row>
-    <row r="64" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
@@ -1790,7 +2221,7 @@
       <c r="F64" s="9"/>
       <c r="G64" s="7"/>
     </row>
-    <row r="65" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
@@ -1799,7 +2230,7 @@
       <c r="F65" s="9"/>
       <c r="G65" s="7"/>
     </row>
-    <row r="66" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
@@ -1808,7 +2239,7 @@
       <c r="F66" s="9"/>
       <c r="G66" s="7"/>
     </row>
-    <row r="67" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
@@ -1817,7 +2248,7 @@
       <c r="F67" s="9"/>
       <c r="G67" s="7"/>
     </row>
-    <row r="68" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
@@ -1826,7 +2257,7 @@
       <c r="F68" s="9"/>
       <c r="G68" s="7"/>
     </row>
-    <row r="69" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="6"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
@@ -1835,7 +2266,7 @@
       <c r="F69" s="9"/>
       <c r="G69" s="7"/>
     </row>
-    <row r="70" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
@@ -1844,7 +2275,7 @@
       <c r="F70" s="9"/>
       <c r="G70" s="7"/>
     </row>
-    <row r="71" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
@@ -1853,7 +2284,7 @@
       <c r="F71" s="9"/>
       <c r="G71" s="7"/>
     </row>
-    <row r="72" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="6"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
@@ -1862,7 +2293,7 @@
       <c r="F72" s="9"/>
       <c r="G72" s="7"/>
     </row>
-    <row r="73" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
@@ -1871,7 +2302,7 @@
       <c r="F73" s="9"/>
       <c r="G73" s="7"/>
     </row>
-    <row r="74" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="6"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
@@ -1880,7 +2311,7 @@
       <c r="F74" s="9"/>
       <c r="G74" s="7"/>
     </row>
-    <row r="75" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
@@ -1889,7 +2320,7 @@
       <c r="F75" s="9"/>
       <c r="G75" s="7"/>
     </row>
-    <row r="76" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
@@ -1898,7 +2329,7 @@
       <c r="F76" s="9"/>
       <c r="G76" s="7"/>
     </row>
-    <row r="77" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
@@ -1907,7 +2338,7 @@
       <c r="F77" s="9"/>
       <c r="G77" s="7"/>
     </row>
-    <row r="78" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
@@ -1916,7 +2347,7 @@
       <c r="F78" s="9"/>
       <c r="G78" s="7"/>
     </row>
-    <row r="79" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
@@ -1925,7 +2356,7 @@
       <c r="F79" s="9"/>
       <c r="G79" s="7"/>
     </row>
-    <row r="80" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
@@ -1934,7 +2365,7 @@
       <c r="F80" s="9"/>
       <c r="G80" s="7"/>
     </row>
-    <row r="81" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="6"/>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
@@ -1943,7 +2374,7 @@
       <c r="F81" s="9"/>
       <c r="G81" s="7"/>
     </row>
-    <row r="82" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="6"/>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
@@ -1952,7 +2383,7 @@
       <c r="F82" s="9"/>
       <c r="G82" s="7"/>
     </row>
-    <row r="83" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="6"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
@@ -1961,7 +2392,7 @@
       <c r="F83" s="9"/>
       <c r="G83" s="7"/>
     </row>
-    <row r="84" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="6"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
@@ -1970,7 +2401,7 @@
       <c r="F84" s="9"/>
       <c r="G84" s="7"/>
     </row>
-    <row r="85" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="6"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
@@ -1979,7 +2410,7 @@
       <c r="F85" s="9"/>
       <c r="G85" s="7"/>
     </row>
-    <row r="86" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
@@ -1988,7 +2419,7 @@
       <c r="F86" s="9"/>
       <c r="G86" s="7"/>
     </row>
-    <row r="87" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
@@ -1997,7 +2428,7 @@
       <c r="F87" s="9"/>
       <c r="G87" s="7"/>
     </row>
-    <row r="88" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
@@ -2006,7 +2437,7 @@
       <c r="F88" s="9"/>
       <c r="G88" s="7"/>
     </row>
-    <row r="89" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
@@ -2015,7 +2446,7 @@
       <c r="F89" s="9"/>
       <c r="G89" s="7"/>
     </row>
-    <row r="90" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="6"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
@@ -2024,7 +2455,7 @@
       <c r="F90" s="9"/>
       <c r="G90" s="7"/>
     </row>
-    <row r="91" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
@@ -2033,7 +2464,7 @@
       <c r="F91" s="9"/>
       <c r="G91" s="7"/>
     </row>
-    <row r="92" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
@@ -2042,7 +2473,7 @@
       <c r="F92" s="9"/>
       <c r="G92" s="7"/>
     </row>
-    <row r="93" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
@@ -2051,7 +2482,7 @@
       <c r="F93" s="9"/>
       <c r="G93" s="7"/>
     </row>
-    <row r="94" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
@@ -2060,7 +2491,7 @@
       <c r="F94" s="9"/>
       <c r="G94" s="7"/>
     </row>
-    <row r="95" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -2069,7 +2500,7 @@
       <c r="F95" s="9"/>
       <c r="G95" s="7"/>
     </row>
-    <row r="96" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
@@ -2078,7 +2509,7 @@
       <c r="F96" s="9"/>
       <c r="G96" s="7"/>
     </row>
-    <row r="97" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" s="6"/>
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
@@ -2087,7 +2518,7 @@
       <c r="F97" s="9"/>
       <c r="G97" s="7"/>
     </row>
-    <row r="98" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A98" s="6"/>
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
@@ -2096,7 +2527,7 @@
       <c r="F98" s="9"/>
       <c r="G98" s="7"/>
     </row>
-    <row r="99" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" s="6"/>
       <c r="B99" s="6"/>
       <c r="C99" s="6"/>
@@ -2105,7 +2536,7 @@
       <c r="F99" s="9"/>
       <c r="G99" s="7"/>
     </row>
-    <row r="100" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="6"/>
       <c r="B100" s="6"/>
       <c r="C100" s="6"/>
@@ -2114,7 +2545,7 @@
       <c r="F100" s="9"/>
       <c r="G100" s="7"/>
     </row>
-    <row r="101" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A101" s="6"/>
       <c r="B101" s="6"/>
       <c r="C101" s="6"/>
@@ -2123,7 +2554,7 @@
       <c r="F101" s="9"/>
       <c r="G101" s="7"/>
     </row>
-    <row r="102" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A102" s="6"/>
       <c r="B102" s="6"/>
       <c r="C102" s="6"/>
@@ -2132,7 +2563,7 @@
       <c r="F102" s="9"/>
       <c r="G102" s="7"/>
     </row>
-    <row r="103" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A103" s="6"/>
       <c r="B103" s="6"/>
       <c r="C103" s="6"/>
@@ -2141,7 +2572,7 @@
       <c r="F103" s="9"/>
       <c r="G103" s="7"/>
     </row>
-    <row r="104" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" s="6"/>
       <c r="B104" s="6"/>
       <c r="C104" s="6"/>
@@ -2150,7 +2581,7 @@
       <c r="F104" s="9"/>
       <c r="G104" s="7"/>
     </row>
-    <row r="105" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A105" s="6"/>
       <c r="B105" s="6"/>
       <c r="C105" s="6"/>
@@ -2159,7 +2590,7 @@
       <c r="F105" s="9"/>
       <c r="G105" s="7"/>
     </row>
-    <row r="106" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" s="6"/>
       <c r="B106" s="6"/>
       <c r="C106" s="6"/>
@@ -2168,7 +2599,7 @@
       <c r="F106" s="9"/>
       <c r="G106" s="7"/>
     </row>
-    <row r="107" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" s="6"/>
       <c r="B107" s="6"/>
       <c r="C107" s="6"/>
@@ -2177,7 +2608,7 @@
       <c r="F107" s="9"/>
       <c r="G107" s="7"/>
     </row>
-    <row r="108" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A108" s="6"/>
       <c r="B108" s="6"/>
       <c r="C108" s="6"/>
@@ -2186,7 +2617,7 @@
       <c r="F108" s="9"/>
       <c r="G108" s="7"/>
     </row>
-    <row r="109" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" s="6"/>
       <c r="B109" s="6"/>
       <c r="C109" s="6"/>
@@ -2195,7 +2626,7 @@
       <c r="F109" s="9"/>
       <c r="G109" s="7"/>
     </row>
-    <row r="110" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A110" s="6"/>
       <c r="B110" s="6"/>
       <c r="C110" s="6"/>
@@ -2204,7 +2635,7 @@
       <c r="F110" s="9"/>
       <c r="G110" s="7"/>
     </row>
-    <row r="111" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A111" s="6"/>
       <c r="B111" s="6"/>
       <c r="C111" s="6"/>
@@ -2213,7 +2644,7 @@
       <c r="F111" s="9"/>
       <c r="G111" s="7"/>
     </row>
-    <row r="112" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A112" s="6"/>
       <c r="B112" s="6"/>
       <c r="C112" s="6"/>
@@ -2222,7 +2653,7 @@
       <c r="F112" s="9"/>
       <c r="G112" s="7"/>
     </row>
-    <row r="113" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A113" s="6"/>
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
@@ -2231,7 +2662,7 @@
       <c r="F113" s="9"/>
       <c r="G113" s="7"/>
     </row>
-    <row r="114" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A114" s="6"/>
       <c r="B114" s="6"/>
       <c r="C114" s="6"/>
@@ -2240,7 +2671,7 @@
       <c r="F114" s="9"/>
       <c r="G114" s="7"/>
     </row>
-    <row r="115" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A115" s="6"/>
       <c r="B115" s="6"/>
       <c r="C115" s="6"/>
@@ -2249,7 +2680,7 @@
       <c r="F115" s="9"/>
       <c r="G115" s="7"/>
     </row>
-    <row r="116" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" s="6"/>
       <c r="B116" s="6"/>
       <c r="C116" s="6"/>
@@ -2258,7 +2689,7 @@
       <c r="F116" s="9"/>
       <c r="G116" s="7"/>
     </row>
-    <row r="117" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A117" s="6"/>
       <c r="B117" s="6"/>
       <c r="C117" s="6"/>
@@ -2267,7 +2698,7 @@
       <c r="F117" s="9"/>
       <c r="G117" s="7"/>
     </row>
-    <row r="118" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A118" s="6"/>
       <c r="B118" s="6"/>
       <c r="C118" s="6"/>
@@ -2276,7 +2707,7 @@
       <c r="F118" s="9"/>
       <c r="G118" s="7"/>
     </row>
-    <row r="119" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A119" s="6"/>
       <c r="B119" s="6"/>
       <c r="C119" s="6"/>
@@ -2285,7 +2716,7 @@
       <c r="F119" s="9"/>
       <c r="G119" s="7"/>
     </row>
-    <row r="120" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A120" s="6"/>
       <c r="B120" s="6"/>
       <c r="C120" s="6"/>
@@ -2294,7 +2725,7 @@
       <c r="F120" s="9"/>
       <c r="G120" s="7"/>
     </row>
-    <row r="121" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A121" s="6"/>
       <c r="B121" s="6"/>
       <c r="C121" s="6"/>
@@ -2303,7 +2734,7 @@
       <c r="F121" s="9"/>
       <c r="G121" s="7"/>
     </row>
-    <row r="122" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A122" s="6"/>
       <c r="B122" s="6"/>
       <c r="C122" s="6"/>
@@ -2311,42 +2742,6 @@
       <c r="E122" s="9"/>
       <c r="F122" s="9"/>
       <c r="G122" s="7"/>
-    </row>
-    <row r="123" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A123" s="6"/>
-      <c r="B123" s="6"/>
-      <c r="C123" s="6"/>
-      <c r="D123" s="9"/>
-      <c r="E123" s="9"/>
-      <c r="F123" s="9"/>
-      <c r="G123" s="7"/>
-    </row>
-    <row r="124" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A124" s="6"/>
-      <c r="B124" s="6"/>
-      <c r="C124" s="6"/>
-      <c r="D124" s="9"/>
-      <c r="E124" s="9"/>
-      <c r="F124" s="9"/>
-      <c r="G124" s="7"/>
-    </row>
-    <row r="125" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A125" s="6"/>
-      <c r="B125" s="6"/>
-      <c r="C125" s="6"/>
-      <c r="D125" s="9"/>
-      <c r="E125" s="9"/>
-      <c r="F125" s="9"/>
-      <c r="G125" s="7"/>
-    </row>
-    <row r="126" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A126" s="6"/>
-      <c r="B126" s="6"/>
-      <c r="C126" s="6"/>
-      <c r="D126" s="9"/>
-      <c r="E126" s="9"/>
-      <c r="F126" s="9"/>
-      <c r="G126" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>